<commit_message>
Matlab from Python / Verbose now works
</commit_message>
<xml_diff>
--- a/2-Autoencoder.xlsx
+++ b/2-Autoencoder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks_000\Desktop\Mentorship\!GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79393309-F1F7-4BBD-9348-010DE04E2A1C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2746D8D-8F54-476F-8282-05E30959CF02}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19596" windowHeight="6876" xr2:uid="{99A690A1-DC36-4BE8-91E6-05B30DF3FF00}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="89">
   <si>
     <t>Input (168x192)</t>
   </si>
@@ -658,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -747,25 +747,28 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -783,7 +786,28 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -792,11 +816,11 @@
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,8 +948,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95B20431-2F3E-41C3-9AC7-159AD65B76C1}" name="Table1" displayName="Table1" ref="A2:X50" totalsRowShown="0">
-  <autoFilter ref="A2:X50" xr:uid="{25EC06B5-7BE5-45AB-AB2D-042D27E65A83}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95B20431-2F3E-41C3-9AC7-159AD65B76C1}" name="Table1" displayName="Table1" ref="A2:X43" totalsRowShown="0">
+  <autoFilter ref="A2:X43" xr:uid="{25EC06B5-7BE5-45AB-AB2D-042D27E65A83}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{318840A2-746A-4FAB-83D3-41719547BE37}" name="subjects" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{0E806CA2-B16E-4541-973E-8F727A98A57A}" name="per_each" dataDxfId="14"/>
@@ -1320,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A51B62-3CE9-4597-806B-508E76E74799}">
   <dimension ref="A1:BN50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I22" workbookViewId="0">
-      <selection activeCell="Y34" sqref="Y34"/>
+    <sheetView tabSelected="1" topLeftCell="F24" workbookViewId="0">
+      <selection activeCell="W48" sqref="W48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1371,93 +1395,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="61" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="53" t="s">
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="55" t="s">
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="64"/>
-      <c r="T1" s="62" t="s">
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="63"/>
-      <c r="V1" s="67" t="s">
+      <c r="U1" s="64"/>
+      <c r="V1" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="AC1" s="53" t="s">
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="AC1" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="55" t="s">
+      <c r="AD1" s="68"/>
+      <c r="AE1" s="68"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="68"/>
+      <c r="AI1" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="55"/>
-      <c r="AK1" s="55"/>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="55"/>
-      <c r="AN1" s="65" t="s">
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="65"/>
-      <c r="AP1" s="52" t="s">
+      <c r="AO1" s="73"/>
+      <c r="AP1" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="AQ1" s="52"/>
-      <c r="AS1" s="53" t="s">
+      <c r="AQ1" s="69"/>
+      <c r="AS1" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="66" t="s">
+      <c r="AT1" s="68"/>
+      <c r="AU1" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="AV1" s="66"/>
-      <c r="AW1" s="66"/>
-      <c r="AX1" s="66"/>
-      <c r="AY1" s="56" t="s">
+      <c r="AV1" s="74"/>
+      <c r="AW1" s="74"/>
+      <c r="AX1" s="74"/>
+      <c r="AY1" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="AZ1" s="56"/>
-      <c r="BA1" s="56"/>
-      <c r="BB1" s="56"/>
-      <c r="BC1" s="57" t="s">
+      <c r="AZ1" s="70"/>
+      <c r="BA1" s="70"/>
+      <c r="BB1" s="70"/>
+      <c r="BC1" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="BD1" s="57"/>
-      <c r="BE1" s="57"/>
-      <c r="BF1" s="57"/>
-      <c r="BG1" s="58" t="s">
+      <c r="BD1" s="71"/>
+      <c r="BE1" s="71"/>
+      <c r="BF1" s="71"/>
+      <c r="BG1" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="BH1" s="58"/>
-      <c r="BI1" s="58"/>
-      <c r="BJ1" s="58"/>
+      <c r="BH1" s="72"/>
+      <c r="BI1" s="72"/>
+      <c r="BJ1" s="72"/>
       <c r="BK1" t="s">
         <v>81</v>
       </c>
@@ -1575,8 +1599,8 @@
       <c r="AO2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="AP2" s="52"/>
-      <c r="AQ2" s="52"/>
+      <c r="AP2" s="69"/>
+      <c r="AQ2" s="69"/>
       <c r="AS2" t="s">
         <v>51</v>
       </c>
@@ -3238,11 +3262,11 @@
         <f t="shared" si="7"/>
         <v>0.98581560283687908</v>
       </c>
-      <c r="BK11" s="52" t="s">
+      <c r="BK11" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="BL11" s="52"/>
-      <c r="BM11" s="52"/>
+      <c r="BL11" s="69"/>
+      <c r="BM11" s="69"/>
       <c r="BN11" s="27"/>
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.3">
@@ -3425,9 +3449,9 @@
         <f t="shared" si="7"/>
         <v>0.98652482269503528</v>
       </c>
-      <c r="BK12" s="52"/>
-      <c r="BL12" s="52"/>
-      <c r="BM12" s="52"/>
+      <c r="BK12" s="69"/>
+      <c r="BL12" s="69"/>
+      <c r="BM12" s="69"/>
       <c r="BN12" s="27"/>
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.3">
@@ -3553,9 +3577,9 @@
       <c r="AP13" t="s">
         <v>80</v>
       </c>
-      <c r="BK13" s="52"/>
-      <c r="BL13" s="52"/>
-      <c r="BM13" s="52"/>
+      <c r="BK13" s="69"/>
+      <c r="BL13" s="69"/>
+      <c r="BM13" s="69"/>
       <c r="BN13" s="27"/>
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.3">
@@ -3681,9 +3705,9 @@
       <c r="AP14" t="s">
         <v>47</v>
       </c>
-      <c r="BK14" s="52"/>
-      <c r="BL14" s="52"/>
-      <c r="BM14" s="52"/>
+      <c r="BK14" s="69"/>
+      <c r="BL14" s="69"/>
+      <c r="BM14" s="69"/>
       <c r="BN14" s="27"/>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.3">
@@ -5480,16 +5504,16 @@
       <c r="H31" s="4">
         <v>0.99617021276595696</v>
       </c>
-      <c r="I31" s="22">
+      <c r="I31" s="52">
         <v>0.08</v>
       </c>
-      <c r="J31" s="22" t="s">
+      <c r="J31" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="K31" s="22">
+      <c r="K31" s="53">
         <v>101</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L31" s="54">
         <v>2.6032142341136902E-3</v>
       </c>
       <c r="M31" s="11" t="s">
@@ -5501,13 +5525,13 @@
       <c r="O31" s="11">
         <v>1E-3</v>
       </c>
-      <c r="P31" s="11">
+      <c r="P31" s="29">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="Q31" s="11" t="s">
+      <c r="Q31" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="R31" s="11">
+      <c r="R31" s="31">
         <v>101</v>
       </c>
       <c r="S31" s="4">
@@ -5536,7 +5560,7 @@
       <c r="AG31" s="20"/>
       <c r="AK31" s="20"/>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7">
         <v>38</v>
       </c>
@@ -5562,16 +5586,16 @@
       <c r="H32" s="8">
         <v>0.99617021276595696</v>
       </c>
-      <c r="I32" s="22">
+      <c r="I32" s="55">
         <v>0.08</v>
       </c>
-      <c r="J32" s="22" t="s">
+      <c r="J32" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="K32" s="22">
+      <c r="K32" s="56">
         <v>10001</v>
       </c>
-      <c r="L32" s="8">
+      <c r="L32" s="57">
         <v>2.3053798358887399E-3</v>
       </c>
       <c r="M32" s="10" t="s">
@@ -5583,13 +5607,13 @@
       <c r="O32" s="10">
         <v>1E-3</v>
       </c>
-      <c r="P32" s="10">
+      <c r="P32" s="38">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="Q32" s="10" t="s">
+      <c r="Q32" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="R32" s="10">
+      <c r="R32" s="40">
         <v>1001</v>
       </c>
       <c r="S32" s="8">
@@ -5674,10 +5698,10 @@
       <c r="S33" s="4">
         <v>1.27289514057338E-3</v>
       </c>
-      <c r="T33" s="15">
+      <c r="T33" s="41">
         <v>18</v>
       </c>
-      <c r="U33" s="15">
+      <c r="U33" s="42">
         <v>6</v>
       </c>
       <c r="V33">
@@ -5753,10 +5777,10 @@
       <c r="S34" s="8">
         <v>1.27289514057338E-3</v>
       </c>
-      <c r="T34" s="16">
+      <c r="T34" s="43">
         <v>18</v>
       </c>
-      <c r="U34" s="16">
+      <c r="U34" s="44">
         <v>16</v>
       </c>
       <c r="V34">
@@ -5832,8 +5856,21 @@
       <c r="S35" s="4">
         <v>1.27289514057338E-3</v>
       </c>
-      <c r="T35" s="15"/>
-      <c r="U35" s="15"/>
+      <c r="T35" s="45">
+        <v>18</v>
+      </c>
+      <c r="U35" s="46">
+        <v>20</v>
+      </c>
+      <c r="V35">
+        <v>0.95914893617021202</v>
+      </c>
+      <c r="W35">
+        <v>0.98979434758557905</v>
+      </c>
+      <c r="X35">
+        <v>0.96212114731615295</v>
+      </c>
       <c r="AB35"/>
       <c r="AF35"/>
       <c r="AG35" s="20"/>
@@ -5898,8 +5935,21 @@
       <c r="S36" s="8">
         <v>1.27289514057338E-3</v>
       </c>
-      <c r="T36" s="16"/>
-      <c r="U36" s="16"/>
+      <c r="T36" s="43">
+        <v>18</v>
+      </c>
+      <c r="U36" s="44">
+        <v>18</v>
+      </c>
+      <c r="V36">
+        <v>0.96042553191489299</v>
+      </c>
+      <c r="W36">
+        <v>0.98981952178474397</v>
+      </c>
+      <c r="X36">
+        <v>0.96194736695197103</v>
+      </c>
       <c r="AB36"/>
       <c r="AF36"/>
       <c r="AG36" s="20"/>
@@ -5931,10 +5981,18 @@
       <c r="H37" s="4">
         <v>0.99617021276595696</v>
       </c>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="4"/>
+      <c r="I37" s="22">
+        <v>0.08</v>
+      </c>
+      <c r="J37" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="K37" s="22">
+        <v>10001</v>
+      </c>
+      <c r="L37" s="4">
+        <v>2.3053798358887399E-3</v>
+      </c>
       <c r="M37" s="11" t="s">
         <v>20</v>
       </c>
@@ -5944,12 +6002,33 @@
       <c r="O37" s="11">
         <v>1E-3</v>
       </c>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="15"/>
-      <c r="U37" s="15"/>
+      <c r="P37" s="11">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Q37" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="R37" s="11">
+        <v>1001</v>
+      </c>
+      <c r="S37" s="4">
+        <v>1.27289514057338E-3</v>
+      </c>
+      <c r="T37" s="45">
+        <v>16</v>
+      </c>
+      <c r="U37" s="46">
+        <v>16</v>
+      </c>
+      <c r="V37">
+        <v>0.98765957446808506</v>
+      </c>
+      <c r="W37">
+        <v>0.98955904552621898</v>
+      </c>
+      <c r="X37">
+        <v>0.97714596851658597</v>
+      </c>
       <c r="AB37"/>
       <c r="AF37"/>
       <c r="AG37" s="20"/>
@@ -5981,10 +6060,18 @@
       <c r="H38" s="8">
         <v>0.99617021276595696</v>
       </c>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="8"/>
+      <c r="I38" s="22">
+        <v>0.08</v>
+      </c>
+      <c r="J38" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="K38" s="22">
+        <v>10001</v>
+      </c>
+      <c r="L38" s="8">
+        <v>2.3053798358887399E-3</v>
+      </c>
       <c r="M38" s="10" t="s">
         <v>20</v>
       </c>
@@ -5994,12 +6081,33 @@
       <c r="O38" s="10">
         <v>1E-3</v>
       </c>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10"/>
-      <c r="S38" s="8"/>
-      <c r="T38" s="16"/>
-      <c r="U38" s="16"/>
+      <c r="P38" s="10">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Q38" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="R38" s="10">
+        <v>1001</v>
+      </c>
+      <c r="S38" s="8">
+        <v>1.27289514057338E-3</v>
+      </c>
+      <c r="T38" s="43">
+        <v>20</v>
+      </c>
+      <c r="U38" s="44">
+        <v>16</v>
+      </c>
+      <c r="V38">
+        <v>0.99872340425531902</v>
+      </c>
+      <c r="W38">
+        <v>0.99817514613986102</v>
+      </c>
+      <c r="X38">
+        <v>0.99732966557213898</v>
+      </c>
       <c r="AB38"/>
       <c r="AF38"/>
       <c r="AG38" s="20"/>
@@ -6031,10 +6139,18 @@
       <c r="H39" s="4">
         <v>0.99617021276595696</v>
       </c>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="4"/>
+      <c r="I39" s="22">
+        <v>0.08</v>
+      </c>
+      <c r="J39" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="K39" s="22">
+        <v>10001</v>
+      </c>
+      <c r="L39" s="4">
+        <v>2.3053798358887399E-3</v>
+      </c>
       <c r="M39" s="11" t="s">
         <v>20</v>
       </c>
@@ -6044,12 +6160,33 @@
       <c r="O39" s="11">
         <v>1E-3</v>
       </c>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="4"/>
-      <c r="T39" s="15"/>
-      <c r="U39" s="15"/>
+      <c r="P39" s="11">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Q39" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="R39" s="11">
+        <v>1001</v>
+      </c>
+      <c r="S39" s="4">
+        <v>1.27289514057338E-3</v>
+      </c>
+      <c r="T39" s="45">
+        <v>22</v>
+      </c>
+      <c r="U39" s="46">
+        <v>16</v>
+      </c>
+      <c r="V39">
+        <v>0.95617021276595704</v>
+      </c>
+      <c r="W39">
+        <v>0.98694173763647397</v>
+      </c>
+      <c r="X39">
+        <v>0.95676194111851498</v>
+      </c>
       <c r="AB39"/>
       <c r="AF39"/>
       <c r="AG39" s="20"/>
@@ -6081,10 +6218,18 @@
       <c r="H40" s="8">
         <v>0.99617021276595696</v>
       </c>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="8"/>
+      <c r="I40" s="22">
+        <v>0.08</v>
+      </c>
+      <c r="J40" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="K40" s="22">
+        <v>10001</v>
+      </c>
+      <c r="L40" s="8">
+        <v>2.3053798358887399E-3</v>
+      </c>
       <c r="M40" s="10" t="s">
         <v>20</v>
       </c>
@@ -6094,12 +6239,33 @@
       <c r="O40" s="10">
         <v>1E-3</v>
       </c>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="16"/>
-      <c r="U40" s="16"/>
+      <c r="P40" s="10">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Q40" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="R40" s="10">
+        <v>1001</v>
+      </c>
+      <c r="S40" s="8">
+        <v>1.27289514057338E-3</v>
+      </c>
+      <c r="T40" s="43">
+        <v>19</v>
+      </c>
+      <c r="U40" s="44">
+        <v>16</v>
+      </c>
+      <c r="V40">
+        <v>0.95914893617021202</v>
+      </c>
+      <c r="W40">
+        <v>0.99003194636358205</v>
+      </c>
+      <c r="X40">
+        <v>0.96274945878929896</v>
+      </c>
       <c r="AB40"/>
       <c r="AF40"/>
       <c r="AG40" s="20"/>
@@ -6131,10 +6297,18 @@
       <c r="H41" s="4">
         <v>0.99617021276595696</v>
       </c>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="4"/>
+      <c r="I41" s="22">
+        <v>0.08</v>
+      </c>
+      <c r="J41" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="K41" s="22">
+        <v>10001</v>
+      </c>
+      <c r="L41" s="4">
+        <v>2.3053798358887399E-3</v>
+      </c>
       <c r="M41" s="11" t="s">
         <v>20</v>
       </c>
@@ -6144,12 +6318,33 @@
       <c r="O41" s="11">
         <v>1E-3</v>
       </c>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="4"/>
-      <c r="T41" s="15"/>
-      <c r="U41" s="15"/>
+      <c r="P41" s="11">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Q41" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="R41" s="11">
+        <v>1001</v>
+      </c>
+      <c r="S41" s="4">
+        <v>1.27289514057338E-3</v>
+      </c>
+      <c r="T41" s="45">
+        <v>20</v>
+      </c>
+      <c r="U41" s="46">
+        <v>18</v>
+      </c>
+      <c r="V41">
+        <v>0.95106382978723403</v>
+      </c>
+      <c r="W41">
+        <v>0.98312447933110003</v>
+      </c>
+      <c r="X41">
+        <v>0.94862178622500504</v>
+      </c>
       <c r="AB41"/>
       <c r="AF41"/>
       <c r="AG41" s="20"/>
@@ -6181,10 +6376,18 @@
       <c r="H42" s="8">
         <v>0.99617021276595696</v>
       </c>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="8"/>
+      <c r="I42" s="22">
+        <v>0.08</v>
+      </c>
+      <c r="J42" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="K42" s="22">
+        <v>10001</v>
+      </c>
+      <c r="L42" s="8">
+        <v>2.3053798358887399E-3</v>
+      </c>
       <c r="M42" s="10" t="s">
         <v>20</v>
       </c>
@@ -6194,18 +6397,39 @@
       <c r="O42" s="10">
         <v>1E-3</v>
       </c>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="10"/>
-      <c r="R42" s="10"/>
-      <c r="S42" s="8"/>
-      <c r="T42" s="16"/>
-      <c r="U42" s="16"/>
+      <c r="P42" s="10">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Q42" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="R42" s="10">
+        <v>1001</v>
+      </c>
+      <c r="S42" s="8">
+        <v>1.27289514057338E-3</v>
+      </c>
+      <c r="T42" s="43">
+        <v>20</v>
+      </c>
+      <c r="U42" s="44">
+        <v>14</v>
+      </c>
+      <c r="V42">
+        <v>0.95787234042553104</v>
+      </c>
+      <c r="W42">
+        <v>0.98912713896856097</v>
+      </c>
+      <c r="X42">
+        <v>0.96093547641863397</v>
+      </c>
       <c r="AB42"/>
       <c r="AF42"/>
       <c r="AG42" s="20"/>
       <c r="AK42" s="20"/>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>38</v>
       </c>
@@ -6231,10 +6455,18 @@
       <c r="H43" s="4">
         <v>0.99617021276595696</v>
       </c>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="4"/>
+      <c r="I43" s="22">
+        <v>0.08</v>
+      </c>
+      <c r="J43" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="K43" s="22">
+        <v>10001</v>
+      </c>
+      <c r="L43" s="4">
+        <v>2.3053798358887399E-3</v>
+      </c>
       <c r="M43" s="11" t="s">
         <v>20</v>
       </c>
@@ -6244,362 +6476,75 @@
       <c r="O43" s="11">
         <v>1E-3</v>
       </c>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
-      <c r="S43" s="4"/>
-      <c r="T43" s="15"/>
-      <c r="U43" s="15"/>
+      <c r="P43" s="11">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Q43" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="R43" s="11">
+        <v>1001</v>
+      </c>
+      <c r="S43" s="4">
+        <v>1.27289514057338E-3</v>
+      </c>
+      <c r="T43" s="75">
+        <v>19.5</v>
+      </c>
+      <c r="U43" s="76">
+        <v>16</v>
+      </c>
+      <c r="V43">
+        <v>0.99872340425531902</v>
+      </c>
+      <c r="W43">
+        <v>0.99817514613986102</v>
+      </c>
+      <c r="X43">
+        <v>0.99732966557213898</v>
+      </c>
       <c r="AB43"/>
       <c r="AF43"/>
       <c r="AG43" s="20"/>
       <c r="AK43" s="20"/>
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A44" s="7">
-        <v>38</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="8">
-        <f>MIN(Table1[[#This Row],[per_each]],64)*Table1[[#This Row],[subjects]]</f>
-        <v>2432</v>
-      </c>
-      <c r="D44" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F44" s="13">
-        <v>20</v>
-      </c>
-      <c r="G44" s="13">
-        <v>6</v>
-      </c>
-      <c r="H44" s="8">
-        <v>0.99617021276595696</v>
-      </c>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="N44" s="10">
-        <v>1E-4</v>
-      </c>
-      <c r="O44" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-      <c r="S44" s="8"/>
-      <c r="T44" s="16"/>
-      <c r="U44" s="16"/>
       <c r="AB44"/>
       <c r="AF44"/>
       <c r="AG44" s="20"/>
       <c r="AK44" s="20"/>
     </row>
     <row r="45" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A45" s="3">
-        <v>38</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" s="4">
-        <f>MIN(Table1[[#This Row],[per_each]],64)*Table1[[#This Row],[subjects]]</f>
-        <v>2432</v>
-      </c>
-      <c r="D45" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F45" s="12">
-        <v>20</v>
-      </c>
-      <c r="G45" s="12">
-        <v>6</v>
-      </c>
-      <c r="H45" s="4">
-        <v>0.99617021276595696</v>
-      </c>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="N45" s="11">
-        <v>1E-4</v>
-      </c>
-      <c r="O45" s="11">
-        <v>1E-3</v>
-      </c>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-      <c r="S45" s="4"/>
-      <c r="T45" s="15"/>
-      <c r="U45" s="15"/>
       <c r="AB45"/>
       <c r="AF45"/>
       <c r="AG45" s="20"/>
       <c r="AK45" s="20"/>
     </row>
     <row r="46" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A46" s="7">
-        <v>38</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="8">
-        <f>MIN(Table1[[#This Row],[per_each]],64)*Table1[[#This Row],[subjects]]</f>
-        <v>2432</v>
-      </c>
-      <c r="D46" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F46" s="13">
-        <v>20</v>
-      </c>
-      <c r="G46" s="13">
-        <v>6</v>
-      </c>
-      <c r="H46" s="8">
-        <v>0.99617021276595696</v>
-      </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="N46" s="10">
-        <v>1E-4</v>
-      </c>
-      <c r="O46" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="P46" s="10"/>
-      <c r="Q46" s="10"/>
-      <c r="R46" s="10"/>
-      <c r="S46" s="8"/>
-      <c r="T46" s="16"/>
-      <c r="U46" s="16"/>
       <c r="AB46"/>
       <c r="AF46"/>
       <c r="AG46" s="20"/>
       <c r="AK46" s="20"/>
     </row>
     <row r="47" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A47" s="3">
-        <v>38</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="4">
-        <f>MIN(Table1[[#This Row],[per_each]],64)*Table1[[#This Row],[subjects]]</f>
-        <v>2432</v>
-      </c>
-      <c r="D47" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F47" s="12">
-        <v>20</v>
-      </c>
-      <c r="G47" s="12">
-        <v>6</v>
-      </c>
-      <c r="H47" s="4">
-        <v>0.99617021276595696</v>
-      </c>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
-      <c r="K47" s="22"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="N47" s="11">
-        <v>1E-4</v>
-      </c>
-      <c r="O47" s="11">
-        <v>1E-3</v>
-      </c>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-      <c r="S47" s="4"/>
-      <c r="T47" s="15"/>
-      <c r="U47" s="15"/>
       <c r="AB47"/>
       <c r="AF47"/>
       <c r="AG47" s="20"/>
       <c r="AK47" s="20"/>
     </row>
     <row r="48" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A48" s="7">
-        <v>38</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="8">
-        <f>MIN(Table1[[#This Row],[per_each]],64)*Table1[[#This Row],[subjects]]</f>
-        <v>2432</v>
-      </c>
-      <c r="D48" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F48" s="13">
-        <v>20</v>
-      </c>
-      <c r="G48" s="13">
-        <v>6</v>
-      </c>
-      <c r="H48" s="8">
-        <v>0.99617021276595696</v>
-      </c>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="N48" s="10">
-        <v>1E-4</v>
-      </c>
-      <c r="O48" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="10"/>
-      <c r="R48" s="10"/>
-      <c r="S48" s="8"/>
-      <c r="T48" s="16"/>
-      <c r="U48" s="16"/>
       <c r="AB48"/>
       <c r="AF48"/>
       <c r="AG48" s="20"/>
       <c r="AK48" s="20"/>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A49" s="3">
-        <v>38</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="4">
-        <f>MIN(Table1[[#This Row],[per_each]],64)*Table1[[#This Row],[subjects]]</f>
-        <v>2432</v>
-      </c>
-      <c r="D49" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F49" s="12">
-        <v>20</v>
-      </c>
-      <c r="G49" s="12">
-        <v>6</v>
-      </c>
-      <c r="H49" s="4">
-        <v>0.99617021276595696</v>
-      </c>
-      <c r="I49" s="22"/>
-      <c r="J49" s="22"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="N49" s="11">
-        <v>1E-4</v>
-      </c>
-      <c r="O49" s="11">
-        <v>1E-3</v>
-      </c>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="4"/>
-      <c r="T49" s="15"/>
-      <c r="U49" s="15"/>
+    <row r="49" spans="28:37" x14ac:dyDescent="0.3">
       <c r="AB49"/>
       <c r="AF49"/>
       <c r="AG49" s="20"/>
       <c r="AK49" s="20"/>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A50" s="7">
-        <v>38</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="8">
-        <f>MIN(Table1[[#This Row],[per_each]],64)*Table1[[#This Row],[subjects]]</f>
-        <v>2432</v>
-      </c>
-      <c r="D50" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F50" s="13">
-        <v>20</v>
-      </c>
-      <c r="G50" s="13">
-        <v>6</v>
-      </c>
-      <c r="H50" s="8">
-        <v>0.99617021276595696</v>
-      </c>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="N50" s="10">
-        <v>1E-4</v>
-      </c>
-      <c r="O50" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="10"/>
-      <c r="R50" s="10"/>
-      <c r="S50" s="8"/>
-      <c r="T50" s="16"/>
-      <c r="U50" s="16"/>
+    <row r="50" spans="28:37" x14ac:dyDescent="0.3">
       <c r="AB50"/>
       <c r="AF50"/>
       <c r="AG50" s="20"/>
@@ -6607,12 +6552,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="M1:S1"/>
-    <mergeCell ref="I1:L1"/>
     <mergeCell ref="BK11:BM14"/>
     <mergeCell ref="AC1:AH1"/>
     <mergeCell ref="AI1:AM1"/>
@@ -6623,8 +6562,14 @@
     <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="AS1:AT1"/>
     <mergeCell ref="AU1:AX1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="M1:S1"/>
+    <mergeCell ref="I1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="V3:V50">
+  <conditionalFormatting sqref="V3:V43">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -6636,7 +6581,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W3:W50">
+  <conditionalFormatting sqref="W3:W43">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -6648,7 +6593,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X3:X50">
+  <conditionalFormatting sqref="X3:X43">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Concatenated into single file
</commit_message>
<xml_diff>
--- a/2-Autoencoder.xlsx
+++ b/2-Autoencoder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks_000\Desktop\Mentorship\!GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2746D8D-8F54-476F-8282-05E30959CF02}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFD9383-9227-47D3-AB74-0EDE278E10CC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19596" windowHeight="6876" xr2:uid="{99A690A1-DC36-4BE8-91E6-05B30DF3FF00}"/>
   </bookViews>
@@ -765,6 +765,39 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -786,41 +819,8 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1344,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A51B62-3CE9-4597-806B-508E76E74799}">
   <dimension ref="A1:BN50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F24" workbookViewId="0">
-      <selection activeCell="W48" sqref="W48"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1395,93 +1395,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="67" t="s">
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="65" t="s">
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="63" t="s">
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="64"/>
-      <c r="V1" s="58" t="s">
+      <c r="U1" s="75"/>
+      <c r="V1" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="AC1" s="67" t="s">
+      <c r="W1" s="70"/>
+      <c r="X1" s="70"/>
+      <c r="AC1" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="68"/>
-      <c r="AF1" s="68"/>
-      <c r="AG1" s="68"/>
-      <c r="AH1" s="68"/>
-      <c r="AI1" s="65" t="s">
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="65"/>
-      <c r="AK1" s="65"/>
-      <c r="AL1" s="65"/>
-      <c r="AM1" s="65"/>
-      <c r="AN1" s="73" t="s">
+      <c r="AJ1" s="63"/>
+      <c r="AK1" s="63"/>
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="73"/>
-      <c r="AP1" s="69" t="s">
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="AQ1" s="69"/>
-      <c r="AS1" s="67" t="s">
+      <c r="AQ1" s="60"/>
+      <c r="AS1" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="AT1" s="68"/>
-      <c r="AU1" s="74" t="s">
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="AV1" s="74"/>
-      <c r="AW1" s="74"/>
-      <c r="AX1" s="74"/>
-      <c r="AY1" s="70" t="s">
+      <c r="AV1" s="68"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="68"/>
+      <c r="AY1" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="AZ1" s="70"/>
-      <c r="BA1" s="70"/>
-      <c r="BB1" s="70"/>
-      <c r="BC1" s="71" t="s">
+      <c r="AZ1" s="64"/>
+      <c r="BA1" s="64"/>
+      <c r="BB1" s="64"/>
+      <c r="BC1" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="BD1" s="71"/>
-      <c r="BE1" s="71"/>
-      <c r="BF1" s="71"/>
-      <c r="BG1" s="72" t="s">
+      <c r="BD1" s="65"/>
+      <c r="BE1" s="65"/>
+      <c r="BF1" s="65"/>
+      <c r="BG1" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="BH1" s="72"/>
-      <c r="BI1" s="72"/>
-      <c r="BJ1" s="72"/>
+      <c r="BH1" s="66"/>
+      <c r="BI1" s="66"/>
+      <c r="BJ1" s="66"/>
       <c r="BK1" t="s">
         <v>81</v>
       </c>
@@ -1599,8 +1599,8 @@
       <c r="AO2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="AP2" s="69"/>
-      <c r="AQ2" s="69"/>
+      <c r="AP2" s="60"/>
+      <c r="AQ2" s="60"/>
       <c r="AS2" t="s">
         <v>51</v>
       </c>
@@ -3262,11 +3262,11 @@
         <f t="shared" si="7"/>
         <v>0.98581560283687908</v>
       </c>
-      <c r="BK11" s="69" t="s">
+      <c r="BK11" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="BL11" s="69"/>
-      <c r="BM11" s="69"/>
+      <c r="BL11" s="60"/>
+      <c r="BM11" s="60"/>
       <c r="BN11" s="27"/>
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.3">
@@ -3449,9 +3449,9 @@
         <f t="shared" si="7"/>
         <v>0.98652482269503528</v>
       </c>
-      <c r="BK12" s="69"/>
-      <c r="BL12" s="69"/>
-      <c r="BM12" s="69"/>
+      <c r="BK12" s="60"/>
+      <c r="BL12" s="60"/>
+      <c r="BM12" s="60"/>
       <c r="BN12" s="27"/>
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.3">
@@ -3577,9 +3577,9 @@
       <c r="AP13" t="s">
         <v>80</v>
       </c>
-      <c r="BK13" s="69"/>
-      <c r="BL13" s="69"/>
-      <c r="BM13" s="69"/>
+      <c r="BK13" s="60"/>
+      <c r="BL13" s="60"/>
+      <c r="BM13" s="60"/>
       <c r="BN13" s="27"/>
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.3">
@@ -3705,9 +3705,9 @@
       <c r="AP14" t="s">
         <v>47</v>
       </c>
-      <c r="BK14" s="69"/>
-      <c r="BL14" s="69"/>
-      <c r="BM14" s="69"/>
+      <c r="BK14" s="60"/>
+      <c r="BL14" s="60"/>
+      <c r="BM14" s="60"/>
       <c r="BN14" s="27"/>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.3">
@@ -6488,10 +6488,10 @@
       <c r="S43" s="4">
         <v>1.27289514057338E-3</v>
       </c>
-      <c r="T43" s="75">
+      <c r="T43" s="58">
         <v>19.5</v>
       </c>
-      <c r="U43" s="76">
+      <c r="U43" s="59">
         <v>16</v>
       </c>
       <c r="V43">
@@ -6552,6 +6552,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="M1:S1"/>
+    <mergeCell ref="I1:L1"/>
     <mergeCell ref="BK11:BM14"/>
     <mergeCell ref="AC1:AH1"/>
     <mergeCell ref="AI1:AM1"/>
@@ -6562,12 +6568,6 @@
     <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="AS1:AT1"/>
     <mergeCell ref="AU1:AX1"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="M1:S1"/>
-    <mergeCell ref="I1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="V3:V43">
     <cfRule type="colorScale" priority="10">

</xml_diff>

<commit_message>
Various fixes * full_model calls seeded properly, return identical results * Fixed memory leak related to uncleared tensorflow graphs * Added proper copying of SDA weights upon creation, encoder-decoder pairs no longer have to be equal
</commit_message>
<xml_diff>
--- a/2-Autoencoder.xlsx
+++ b/2-Autoencoder.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks_000\Desktop\Mentorship\!GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D33AC75-0A06-4251-8359-394DD969D9AF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E05253-131C-42CF-9E0B-F7D84F2EA126}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19596" windowHeight="6876" xr2:uid="{99A690A1-DC36-4BE8-91E6-05B30DF3FF00}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="90">
   <si>
     <t>Input (168x192)</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>AE loss1-a</t>
+  </si>
+  <si>
+    <t>&lt; Sda nonequal weights</t>
   </si>
 </sst>
 </file>
@@ -771,6 +774,33 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -792,34 +822,7 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1344,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A51B62-3CE9-4597-806B-508E76E74799}">
   <dimension ref="A1:BN50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="BH2" sqref="BH2"/>
+    <sheetView tabSelected="1" topLeftCell="U32" workbookViewId="0">
+      <selection activeCell="AA43" sqref="AA43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1395,93 +1398,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="64" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="69" t="s">
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="67" t="s">
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="65" t="s">
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="66"/>
-      <c r="V1" s="60" t="s">
+      <c r="U1" s="75"/>
+      <c r="V1" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="AC1" s="69" t="s">
+      <c r="W1" s="70"/>
+      <c r="X1" s="70"/>
+      <c r="AC1" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="70"/>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="70"/>
-      <c r="AG1" s="70"/>
-      <c r="AH1" s="70"/>
-      <c r="AI1" s="67" t="s">
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="67"/>
-      <c r="AK1" s="67"/>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="75" t="s">
+      <c r="AJ1" s="63"/>
+      <c r="AK1" s="63"/>
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="75"/>
-      <c r="AP1" s="71" t="s">
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="AQ1" s="71"/>
-      <c r="AS1" s="69" t="s">
+      <c r="AQ1" s="60"/>
+      <c r="AS1" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="AT1" s="70"/>
-      <c r="AU1" s="76" t="s">
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="AV1" s="76"/>
-      <c r="AW1" s="76"/>
-      <c r="AX1" s="76"/>
-      <c r="AY1" s="72" t="s">
+      <c r="AV1" s="68"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="68"/>
+      <c r="AY1" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="AZ1" s="72"/>
-      <c r="BA1" s="72"/>
-      <c r="BB1" s="72"/>
-      <c r="BC1" s="73" t="s">
+      <c r="AZ1" s="64"/>
+      <c r="BA1" s="64"/>
+      <c r="BB1" s="64"/>
+      <c r="BC1" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="BD1" s="73"/>
-      <c r="BE1" s="73"/>
-      <c r="BF1" s="73"/>
-      <c r="BG1" s="74" t="s">
+      <c r="BD1" s="65"/>
+      <c r="BE1" s="65"/>
+      <c r="BF1" s="65"/>
+      <c r="BG1" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="BH1" s="74"/>
-      <c r="BI1" s="74"/>
-      <c r="BJ1" s="74"/>
+      <c r="BH1" s="66"/>
+      <c r="BI1" s="66"/>
+      <c r="BJ1" s="66"/>
       <c r="BK1" t="s">
         <v>79</v>
       </c>
@@ -1599,8 +1602,8 @@
       <c r="AO2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="AP2" s="71"/>
-      <c r="AQ2" s="71"/>
+      <c r="AP2" s="60"/>
+      <c r="AQ2" s="60"/>
       <c r="AS2" t="s">
         <v>51</v>
       </c>
@@ -3262,11 +3265,11 @@
         <f t="shared" si="7"/>
         <v>0.98581560283687908</v>
       </c>
-      <c r="BK11" s="71" t="s">
+      <c r="BK11" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="BL11" s="71"/>
-      <c r="BM11" s="71"/>
+      <c r="BL11" s="60"/>
+      <c r="BM11" s="60"/>
       <c r="BN11" s="27"/>
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.3">
@@ -3449,9 +3452,9 @@
         <f t="shared" si="7"/>
         <v>0.98652482269503528</v>
       </c>
-      <c r="BK12" s="71"/>
-      <c r="BL12" s="71"/>
-      <c r="BM12" s="71"/>
+      <c r="BK12" s="60"/>
+      <c r="BL12" s="60"/>
+      <c r="BM12" s="60"/>
       <c r="BN12" s="27"/>
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.3">
@@ -3577,9 +3580,9 @@
       <c r="AP13" t="s">
         <v>78</v>
       </c>
-      <c r="BK13" s="71"/>
-      <c r="BL13" s="71"/>
-      <c r="BM13" s="71"/>
+      <c r="BK13" s="60"/>
+      <c r="BL13" s="60"/>
+      <c r="BM13" s="60"/>
       <c r="BN13" s="27"/>
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.3">
@@ -3705,9 +3708,9 @@
       <c r="AP14" t="s">
         <v>47</v>
       </c>
-      <c r="BK14" s="71"/>
-      <c r="BL14" s="71"/>
-      <c r="BM14" s="71"/>
+      <c r="BK14" s="60"/>
+      <c r="BL14" s="60"/>
+      <c r="BM14" s="60"/>
       <c r="BN14" s="27"/>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.3">
@@ -6509,6 +6512,9 @@
       <c r="AK43" s="20"/>
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="Y44" t="s">
+        <v>89</v>
+      </c>
       <c r="AB44"/>
       <c r="AF44"/>
       <c r="AG44" s="20"/>
@@ -6552,6 +6558,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="M1:S1"/>
+    <mergeCell ref="I1:L1"/>
     <mergeCell ref="BK11:BM14"/>
     <mergeCell ref="AC1:AH1"/>
     <mergeCell ref="AI1:AM1"/>
@@ -6562,12 +6574,6 @@
     <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="AS1:AT1"/>
     <mergeCell ref="AU1:AX1"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="M1:S1"/>
-    <mergeCell ref="I1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="V3:V43">
     <cfRule type="colorScale" priority="10">

</xml_diff>